<commit_message>
add corals per rack
</commit_message>
<xml_diff>
--- a/data/reproducibility/pam_order.xlsx
+++ b/data/reproducibility/pam_order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrcunning/Projects/CBASS_methods/data/reproducibility/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9C82D5-8525-9043-9C61-A6A031A2527C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B611C42-7D64-B249-8D25-CE3283348A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-31780" yWindow="1880" windowWidth="28040" windowHeight="16940" xr2:uid="{5E9A048C-A98B-BE40-BF65-3E6FF80A44E7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="62">
   <si>
     <t>date</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>2021-09-08</t>
+  </si>
+  <si>
+    <t>n_corals</t>
   </si>
 </sst>
 </file>
@@ -575,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20827370-1184-374B-BE19-A8B422001152}">
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -590,7 +593,7 @@
     <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,8 +606,11 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -617,8 +623,11 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -631,8 +640,11 @@
       <c r="D3" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -645,8 +657,11 @@
       <c r="D4" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -659,8 +674,11 @@
       <c r="D5" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -673,8 +691,11 @@
       <c r="D6" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -687,8 +708,11 @@
       <c r="D7" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -701,8 +725,11 @@
       <c r="D8" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -715,8 +742,11 @@
       <c r="D9" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -729,8 +759,11 @@
       <c r="D10" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -743,8 +776,11 @@
       <c r="D11" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -757,8 +793,11 @@
       <c r="D12" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -771,8 +810,11 @@
       <c r="D13" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -785,8 +827,11 @@
       <c r="D14" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -799,8 +844,11 @@
       <c r="D15" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
@@ -813,8 +861,11 @@
       <c r="D16" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -827,8 +878,11 @@
       <c r="D17" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
@@ -841,8 +895,11 @@
       <c r="D18" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
@@ -855,8 +912,11 @@
       <c r="D19" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
@@ -869,8 +929,11 @@
       <c r="D20" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -883,8 +946,11 @@
       <c r="D21" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
@@ -897,8 +963,11 @@
       <c r="D22" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
@@ -911,8 +980,11 @@
       <c r="D23" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
@@ -925,8 +997,11 @@
       <c r="D24" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>4</v>
       </c>
@@ -939,8 +1014,11 @@
       <c r="D25" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>4</v>
       </c>
@@ -953,8 +1031,11 @@
       <c r="D26" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>4</v>
       </c>
@@ -967,8 +1048,11 @@
       <c r="D27" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>4</v>
       </c>
@@ -981,8 +1065,11 @@
       <c r="D28" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
@@ -995,8 +1082,11 @@
       <c r="D29" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>4</v>
       </c>
@@ -1009,8 +1099,11 @@
       <c r="D30" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>4</v>
       </c>
@@ -1023,8 +1116,11 @@
       <c r="D31" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
@@ -1037,8 +1133,11 @@
       <c r="D32" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -1051,8 +1150,11 @@
       <c r="D33" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>4</v>
       </c>
@@ -1065,8 +1167,11 @@
       <c r="D34" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>4</v>
       </c>
@@ -1079,8 +1184,11 @@
       <c r="D35" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>4</v>
       </c>
@@ -1093,8 +1201,11 @@
       <c r="D36" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>4</v>
       </c>
@@ -1107,8 +1218,11 @@
       <c r="D37" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>4</v>
       </c>
@@ -1121,8 +1235,11 @@
       <c r="D38" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>4</v>
       </c>
@@ -1135,8 +1252,11 @@
       <c r="D39" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>4</v>
       </c>
@@ -1149,8 +1269,11 @@
       <c r="D40" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>4</v>
       </c>
@@ -1163,8 +1286,11 @@
       <c r="D41" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>4</v>
       </c>
@@ -1177,8 +1303,11 @@
       <c r="D42" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>4</v>
       </c>
@@ -1191,8 +1320,11 @@
       <c r="D43" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>4</v>
       </c>
@@ -1205,8 +1337,11 @@
       <c r="D44" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>4</v>
       </c>
@@ -1219,8 +1354,11 @@
       <c r="D45" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>4</v>
       </c>
@@ -1233,8 +1371,11 @@
       <c r="D46" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>4</v>
       </c>
@@ -1247,8 +1388,11 @@
       <c r="D47" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>4</v>
       </c>
@@ -1261,8 +1405,11 @@
       <c r="D48" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>4</v>
       </c>
@@ -1275,8 +1422,11 @@
       <c r="D49" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>4</v>
       </c>
@@ -1289,8 +1439,11 @@
       <c r="D50" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>60</v>
       </c>
@@ -1303,8 +1456,11 @@
       <c r="D51" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>60</v>
       </c>
@@ -1317,8 +1473,11 @@
       <c r="D52" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>60</v>
       </c>
@@ -1331,8 +1490,11 @@
       <c r="D53" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>60</v>
       </c>
@@ -1345,8 +1507,11 @@
       <c r="D54" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>60</v>
       </c>
@@ -1359,8 +1524,11 @@
       <c r="D55" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>60</v>
       </c>
@@ -1373,8 +1541,11 @@
       <c r="D56" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>60</v>
       </c>
@@ -1387,8 +1558,11 @@
       <c r="D57" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>60</v>
       </c>
@@ -1401,8 +1575,11 @@
       <c r="D58" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>60</v>
       </c>
@@ -1415,8 +1592,11 @@
       <c r="D59" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>60</v>
       </c>
@@ -1429,8 +1609,11 @@
       <c r="D60" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
@@ -1443,8 +1626,11 @@
       <c r="D61" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
@@ -1457,8 +1643,11 @@
       <c r="D62" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>60</v>
       </c>
@@ -1471,8 +1660,11 @@
       <c r="D63" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>60</v>
       </c>
@@ -1485,8 +1677,11 @@
       <c r="D64" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>60</v>
       </c>
@@ -1499,8 +1694,11 @@
       <c r="D65" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>60</v>
       </c>
@@ -1513,8 +1711,11 @@
       <c r="D66" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>60</v>
       </c>
@@ -1527,8 +1728,11 @@
       <c r="D67" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>60</v>
       </c>
@@ -1541,8 +1745,11 @@
       <c r="D68" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>60</v>
       </c>
@@ -1555,8 +1762,11 @@
       <c r="D69" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>60</v>
       </c>
@@ -1569,8 +1779,11 @@
       <c r="D70" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>60</v>
       </c>
@@ -1583,8 +1796,11 @@
       <c r="D71" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>60</v>
       </c>
@@ -1597,8 +1813,11 @@
       <c r="D72" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>60</v>
       </c>
@@ -1611,8 +1830,11 @@
       <c r="D73" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>60</v>
       </c>
@@ -1625,8 +1847,11 @@
       <c r="D74" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>60</v>
       </c>
@@ -1639,8 +1864,11 @@
       <c r="D75" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>60</v>
       </c>
@@ -1653,8 +1881,11 @@
       <c r="D76" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>60</v>
       </c>
@@ -1667,8 +1898,11 @@
       <c r="D77" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>60</v>
       </c>
@@ -1681,8 +1915,11 @@
       <c r="D78" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>60</v>
       </c>
@@ -1695,8 +1932,11 @@
       <c r="D79" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>60</v>
       </c>
@@ -1709,8 +1949,11 @@
       <c r="D80" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>60</v>
       </c>
@@ -1723,8 +1966,11 @@
       <c r="D81" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>60</v>
       </c>
@@ -1737,8 +1983,11 @@
       <c r="D82" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E82" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>60</v>
       </c>
@@ -1751,8 +2000,11 @@
       <c r="D83" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E83" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>60</v>
       </c>
@@ -1765,8 +2017,11 @@
       <c r="D84" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E84" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>60</v>
       </c>
@@ -1779,8 +2034,11 @@
       <c r="D85" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E85" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>60</v>
       </c>
@@ -1793,8 +2051,11 @@
       <c r="D86" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E86" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>60</v>
       </c>
@@ -1807,8 +2068,11 @@
       <c r="D87" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E87" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>60</v>
       </c>
@@ -1821,8 +2085,11 @@
       <c r="D88" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E88" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>60</v>
       </c>
@@ -1835,8 +2102,11 @@
       <c r="D89" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E89" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>60</v>
       </c>
@@ -1848,6 +2118,9 @@
       </c>
       <c r="D90" s="1" t="s">
         <v>56</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>